<commit_message>
Fixed Year Column Issue
</commit_message>
<xml_diff>
--- a/Task_Distribution/ques_data.xlsx
+++ b/Task_Distribution/ques_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\Task Distribution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git Repo\Python-projects\Task_Distribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13D5C904-E093-451E-AB49-F30B19E233E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6699FAA-9949-4C8D-B474-26B4BE5EB0CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>2018-19</t>
-  </si>
-  <si>
-    <t>2017-18</t>
-  </si>
-  <si>
-    <t>2015-16</t>
-  </si>
-  <si>
-    <t>2014-15</t>
-  </si>
-  <si>
-    <t>2013-14</t>
-  </si>
-  <si>
     <t>MME213</t>
   </si>
   <si>
@@ -51,11 +36,26 @@
   <si>
     <t>ME221</t>
   </si>
+  <si>
+    <t>2018-19</t>
+  </si>
+  <si>
+    <t>2017-18</t>
+  </si>
+  <si>
+    <t>2016-17</t>
+  </si>
+  <si>
+    <t>2015-16</t>
+  </si>
+  <si>
+    <t>2014-15</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -889,11 +889,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,21 +903,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -934,7 +934,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>12</v>
@@ -951,7 +951,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>12</v>
@@ -968,7 +968,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>12</v>
@@ -985,7 +985,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>12</v>

</xml_diff>

<commit_message>
Added Optional Course sheet
</commit_message>
<xml_diff>
--- a/Task_Distribution/ques_data.xlsx
+++ b/Task_Distribution/ques_data.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git Repo\Python-projects\Task_Distribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A934EA-284E-4844-B035-C14F9A478E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB56D79-97CC-4BB9-92A9-B042373D6AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Year</t>
   </si>
@@ -50,6 +51,12 @@
   </si>
   <si>
     <t>2014-15</t>
+  </si>
+  <si>
+    <t>HUM103</t>
+  </si>
+  <si>
+    <t>HUM303</t>
   </si>
 </sst>
 </file>
@@ -892,7 +899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -1003,4 +1010,72 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D28E1C59-02AD-4306-AAD0-0FA578F38ED5}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>58</v>
+      </c>
+      <c r="B6">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>